<commit_message>
soc nu echt gefixt
</commit_message>
<xml_diff>
--- a/BusPlanning.xlsx
+++ b/BusPlanning.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://stichtingfontys-my.sharepoint.com/personal/527924_student_fontys_nl/Documents/Documenten/Project_5/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="28" documentId="8_{536F4F94-487A-4319-A5D9-6382845A77E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7E11527B-44CF-4F8E-88A8-6477409A1265}"/>
+  <xr:revisionPtr revIDLastSave="42" documentId="8_{536F4F94-487A-4319-A5D9-6382845A77E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{79D60E2F-59E4-4F56-82B8-159BDE050358}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="11520" windowHeight="12360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,20 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$H$721</definedName>
   </definedNames>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -2355,10 +2368,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr filterMode="1"/>
-  <dimension ref="A1:H721"/>
+  <dimension ref="A1:I721"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E728" sqref="E728"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="I19" sqref="I19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2367,8 +2380,8 @@
     <col min="2" max="2" width="15.88671875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13.44140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12.88671875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.5546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.44140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.5546875" hidden="1" customWidth="1"/>
+    <col min="6" max="6" width="8.44140625" hidden="1" customWidth="1"/>
     <col min="7" max="7" width="23" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -2424,7 +2437,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>13</v>
       </c>
@@ -2447,7 +2460,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>13</v>
       </c>
@@ -2496,7 +2509,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>9</v>
       </c>
@@ -2519,7 +2532,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>8</v>
       </c>
@@ -2640,7 +2653,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>9</v>
       </c>
@@ -2666,7 +2679,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>13</v>
       </c>
@@ -2738,7 +2751,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>13</v>
       </c>
@@ -2764,7 +2777,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>8</v>
       </c>
@@ -2787,7 +2800,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="18" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>9</v>
       </c>
@@ -2809,8 +2822,12 @@
       <c r="H18">
         <v>1</v>
       </c>
-    </row>
-    <row r="19" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+      <c r="I18">
+        <f>270-G7-G12</f>
+        <v>257.21639999999996</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>9</v>
       </c>
@@ -2836,7 +2853,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>9</v>
       </c>
@@ -2862,7 +2879,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="21" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>13</v>
       </c>
@@ -2885,7 +2902,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="22" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>8</v>
       </c>
@@ -2908,7 +2925,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="23" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>8</v>
       </c>
@@ -2931,7 +2948,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="24" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>13</v>
       </c>
@@ -2954,7 +2971,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>13</v>
       </c>
@@ -2980,7 +2997,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>13</v>
       </c>
@@ -3006,7 +3023,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="27" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>9</v>
       </c>
@@ -3029,7 +3046,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="28" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>8</v>
       </c>
@@ -3052,7 +3069,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="29" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>8</v>
       </c>
@@ -3075,7 +3092,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="30" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>9</v>
       </c>
@@ -3101,7 +3118,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="31" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>13</v>
       </c>
@@ -3124,7 +3141,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="32" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>9</v>
       </c>
@@ -3132,10 +3149,10 @@
         <v>13</v>
       </c>
       <c r="C32" t="s">
-        <v>277</v>
+        <v>22</v>
       </c>
       <c r="D32" t="s">
-        <v>278</v>
+        <v>23</v>
       </c>
       <c r="E32" t="s">
         <v>15</v>
@@ -3147,7 +3164,7 @@
         <v>12.849600000000001</v>
       </c>
       <c r="H32">
-        <v>6</v>
+        <v>1</v>
       </c>
     </row>
     <row r="33" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
@@ -3196,7 +3213,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="35" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>9</v>
       </c>
@@ -3227,10 +3244,10 @@
         <v>13</v>
       </c>
       <c r="C36" t="s">
-        <v>22</v>
+        <v>57</v>
       </c>
       <c r="D36" t="s">
-        <v>23</v>
+        <v>58</v>
       </c>
       <c r="E36" t="s">
         <v>15</v>
@@ -3325,10 +3342,10 @@
         <v>13</v>
       </c>
       <c r="C40" t="s">
-        <v>322</v>
+        <v>95</v>
       </c>
       <c r="D40" t="s">
-        <v>323</v>
+        <v>96</v>
       </c>
       <c r="E40" t="s">
         <v>15</v>
@@ -3340,7 +3357,7 @@
         <v>12.849600000000001</v>
       </c>
       <c r="H40">
-        <v>7</v>
+        <v>2</v>
       </c>
     </row>
     <row r="41" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
@@ -3489,16 +3506,16 @@
     </row>
     <row r="47" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="B47" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="C47" t="s">
-        <v>279</v>
+        <v>120</v>
       </c>
       <c r="D47" t="s">
-        <v>280</v>
+        <v>121</v>
       </c>
       <c r="E47" t="s">
         <v>15</v>
@@ -3507,10 +3524,10 @@
         <v>400</v>
       </c>
       <c r="G47">
-        <v>12.3</v>
+        <v>12.849600000000001</v>
       </c>
       <c r="H47">
-        <v>6</v>
+        <v>2</v>
       </c>
     </row>
     <row r="48" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
@@ -3539,7 +3556,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="49" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>13</v>
       </c>
@@ -3562,7 +3579,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="50" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>13</v>
       </c>
@@ -3757,16 +3774,16 @@
     </row>
     <row r="58" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="B58" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="C58" t="s">
-        <v>324</v>
+        <v>156</v>
       </c>
       <c r="D58" t="s">
-        <v>325</v>
+        <v>157</v>
       </c>
       <c r="E58" t="s">
         <v>15</v>
@@ -3775,10 +3792,10 @@
         <v>400</v>
       </c>
       <c r="G58">
-        <v>12.3</v>
+        <v>12.849600000000001</v>
       </c>
       <c r="H58">
-        <v>7</v>
+        <v>3</v>
       </c>
     </row>
     <row r="59" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
@@ -3812,10 +3829,10 @@
         <v>13</v>
       </c>
       <c r="C60" t="s">
-        <v>154</v>
+        <v>163</v>
       </c>
       <c r="D60" t="s">
-        <v>552</v>
+        <v>164</v>
       </c>
       <c r="E60" t="s">
         <v>15</v>
@@ -3827,7 +3844,7 @@
         <v>12.849600000000001</v>
       </c>
       <c r="H60">
-        <v>15</v>
+        <v>3</v>
       </c>
     </row>
     <row r="61" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
@@ -3974,7 +3991,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="67" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
         <v>9</v>
       </c>
@@ -3999,16 +4016,16 @@
     </row>
     <row r="68" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="B68" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="C68" t="s">
-        <v>372</v>
+        <v>182</v>
       </c>
       <c r="D68" t="s">
-        <v>373</v>
+        <v>183</v>
       </c>
       <c r="E68" t="s">
         <v>15</v>
@@ -4017,10 +4034,10 @@
         <v>400</v>
       </c>
       <c r="G68">
-        <v>12.3</v>
+        <v>12.849600000000001</v>
       </c>
       <c r="H68">
-        <v>8</v>
+        <v>3</v>
       </c>
     </row>
     <row r="69" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
@@ -4051,16 +4068,16 @@
     </row>
     <row r="70" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="B70" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C70" t="s">
-        <v>95</v>
+        <v>192</v>
       </c>
       <c r="D70" t="s">
-        <v>96</v>
+        <v>193</v>
       </c>
       <c r="E70" t="s">
         <v>15</v>
@@ -4069,10 +4086,10 @@
         <v>400</v>
       </c>
       <c r="G70">
-        <v>12.849600000000001</v>
+        <v>12.3</v>
       </c>
       <c r="H70">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="71" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
@@ -4129,10 +4146,10 @@
         <v>13</v>
       </c>
       <c r="C73" t="s">
-        <v>572</v>
+        <v>206</v>
       </c>
       <c r="D73" t="s">
-        <v>326</v>
+        <v>207</v>
       </c>
       <c r="E73" t="s">
         <v>15</v>
@@ -4144,7 +4161,7 @@
         <v>12.849600000000001</v>
       </c>
       <c r="H73">
-        <v>16</v>
+        <v>4</v>
       </c>
     </row>
     <row r="74" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
@@ -4339,16 +4356,16 @@
     </row>
     <row r="82" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="B82" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="C82" t="s">
-        <v>282</v>
+        <v>213</v>
       </c>
       <c r="D82" t="s">
-        <v>283</v>
+        <v>214</v>
       </c>
       <c r="E82" t="s">
         <v>15</v>
@@ -4357,10 +4374,10 @@
         <v>400</v>
       </c>
       <c r="G82">
-        <v>12.3</v>
+        <v>12.849600000000001</v>
       </c>
       <c r="H82">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="83" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
@@ -4371,10 +4388,10 @@
         <v>13</v>
       </c>
       <c r="C83" t="s">
-        <v>247</v>
+        <v>232</v>
       </c>
       <c r="D83" t="s">
-        <v>597</v>
+        <v>233</v>
       </c>
       <c r="E83" t="s">
         <v>15</v>
@@ -4386,10 +4403,10 @@
         <v>12.849600000000001</v>
       </c>
       <c r="H83">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="84" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="84" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
         <v>13</v>
       </c>
@@ -4593,10 +4610,10 @@
         <v>9</v>
       </c>
       <c r="C92" t="s">
-        <v>327</v>
+        <v>234</v>
       </c>
       <c r="D92" t="s">
-        <v>328</v>
+        <v>235</v>
       </c>
       <c r="E92" t="s">
         <v>15</v>
@@ -4608,7 +4625,7 @@
         <v>12.3</v>
       </c>
       <c r="H92">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="93" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
@@ -4662,16 +4679,16 @@
     </row>
     <row r="95" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="B95" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C95" t="s">
-        <v>156</v>
+        <v>237</v>
       </c>
       <c r="D95" t="s">
-        <v>157</v>
+        <v>238</v>
       </c>
       <c r="E95" t="s">
         <v>15</v>
@@ -4680,10 +4697,10 @@
         <v>400</v>
       </c>
       <c r="G95">
-        <v>12.849600000000001</v>
+        <v>12.3</v>
       </c>
       <c r="H95">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="96" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
@@ -4740,10 +4757,10 @@
         <v>13</v>
       </c>
       <c r="C98" t="s">
-        <v>619</v>
+        <v>29</v>
       </c>
       <c r="D98" t="s">
-        <v>284</v>
+        <v>249</v>
       </c>
       <c r="E98" t="s">
         <v>15</v>
@@ -4755,7 +4772,7 @@
         <v>12.849600000000001</v>
       </c>
       <c r="H98">
-        <v>18</v>
+        <v>5</v>
       </c>
     </row>
     <row r="99" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
@@ -4855,16 +4872,16 @@
     </row>
     <row r="103" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A103" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="B103" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="C103" t="s">
-        <v>421</v>
+        <v>268</v>
       </c>
       <c r="D103" t="s">
-        <v>206</v>
+        <v>269</v>
       </c>
       <c r="E103" t="s">
         <v>15</v>
@@ -4873,10 +4890,10 @@
         <v>400</v>
       </c>
       <c r="G103">
-        <v>12.3</v>
+        <v>12.849600000000001</v>
       </c>
       <c r="H103">
-        <v>9</v>
+        <v>5</v>
       </c>
     </row>
     <row r="104" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
@@ -4959,10 +4976,10 @@
         <v>9</v>
       </c>
       <c r="C107" t="s">
-        <v>375</v>
+        <v>270</v>
       </c>
       <c r="D107" t="s">
-        <v>376</v>
+        <v>271</v>
       </c>
       <c r="E107" t="s">
         <v>15</v>
@@ -4974,7 +4991,7 @@
         <v>12.3</v>
       </c>
       <c r="H107">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="108" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
@@ -5002,16 +5019,16 @@
     </row>
     <row r="109" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A109" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="B109" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C109" t="s">
-        <v>27</v>
+        <v>273</v>
       </c>
       <c r="D109" t="s">
-        <v>639</v>
+        <v>274</v>
       </c>
       <c r="E109" t="s">
         <v>15</v>
@@ -5020,13 +5037,13 @@
         <v>400</v>
       </c>
       <c r="G109">
-        <v>12.849600000000001</v>
+        <v>12.3</v>
       </c>
       <c r="H109">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="110" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="110" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A110" t="s">
         <v>9</v>
       </c>
@@ -5195,16 +5212,16 @@
     </row>
     <row r="117" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A117" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="B117" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="C117" t="s">
-        <v>285</v>
+        <v>277</v>
       </c>
       <c r="D117" t="s">
-        <v>286</v>
+        <v>278</v>
       </c>
       <c r="E117" t="s">
         <v>15</v>
@@ -5213,7 +5230,7 @@
         <v>400</v>
       </c>
       <c r="G117">
-        <v>12.3</v>
+        <v>12.849600000000001</v>
       </c>
       <c r="H117">
         <v>6</v>
@@ -5270,16 +5287,16 @@
     </row>
     <row r="120" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A120" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="B120" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C120" t="s">
-        <v>206</v>
+        <v>279</v>
       </c>
       <c r="D120" t="s">
-        <v>207</v>
+        <v>280</v>
       </c>
       <c r="E120" t="s">
         <v>15</v>
@@ -5288,10 +5305,10 @@
         <v>400</v>
       </c>
       <c r="G120">
-        <v>12.849600000000001</v>
+        <v>12.3</v>
       </c>
       <c r="H120">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="121" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
@@ -5342,16 +5359,16 @@
     </row>
     <row r="123" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A123" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="B123" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C123" t="s">
-        <v>574</v>
+        <v>282</v>
       </c>
       <c r="D123" t="s">
-        <v>377</v>
+        <v>283</v>
       </c>
       <c r="E123" t="s">
         <v>15</v>
@@ -5360,10 +5377,10 @@
         <v>400</v>
       </c>
       <c r="G123">
-        <v>12.849600000000001</v>
+        <v>12.3</v>
       </c>
       <c r="H123">
-        <v>16</v>
+        <v>6</v>
       </c>
     </row>
     <row r="124" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
@@ -5389,7 +5406,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="125" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A125" t="s">
         <v>13</v>
       </c>
@@ -5472,10 +5489,10 @@
         <v>9</v>
       </c>
       <c r="C128" t="s">
-        <v>456</v>
+        <v>285</v>
       </c>
       <c r="D128" t="s">
-        <v>29</v>
+        <v>286</v>
       </c>
       <c r="E128" t="s">
         <v>15</v>
@@ -5487,7 +5504,7 @@
         <v>12.3</v>
       </c>
       <c r="H128">
-        <v>10</v>
+        <v>6</v>
       </c>
     </row>
     <row r="129" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
@@ -5570,10 +5587,10 @@
         <v>9</v>
       </c>
       <c r="C132" t="s">
-        <v>330</v>
+        <v>288</v>
       </c>
       <c r="D132" t="s">
-        <v>331</v>
+        <v>289</v>
       </c>
       <c r="E132" t="s">
         <v>15</v>
@@ -5585,7 +5602,7 @@
         <v>12.3</v>
       </c>
       <c r="H132">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="133" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
@@ -5613,16 +5630,16 @@
     </row>
     <row r="134" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A134" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="B134" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C134" t="s">
-        <v>99</v>
+        <v>291</v>
       </c>
       <c r="D134" t="s">
-        <v>599</v>
+        <v>292</v>
       </c>
       <c r="E134" t="s">
         <v>15</v>
@@ -5631,10 +5648,10 @@
         <v>400</v>
       </c>
       <c r="G134">
-        <v>12.849600000000001</v>
+        <v>12.3</v>
       </c>
       <c r="H134">
-        <v>17</v>
+        <v>6</v>
       </c>
     </row>
     <row r="135" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
@@ -5815,10 +5832,10 @@
         <v>9</v>
       </c>
       <c r="C142" t="s">
-        <v>378</v>
+        <v>294</v>
       </c>
       <c r="D142" t="s">
-        <v>379</v>
+        <v>295</v>
       </c>
       <c r="E142" t="s">
         <v>15</v>
@@ -5830,7 +5847,7 @@
         <v>12.3</v>
       </c>
       <c r="H142">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="143" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
@@ -5861,16 +5878,16 @@
     </row>
     <row r="144" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A144" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="B144" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C144" t="s">
-        <v>29</v>
+        <v>297</v>
       </c>
       <c r="D144" t="s">
-        <v>249</v>
+        <v>298</v>
       </c>
       <c r="E144" t="s">
         <v>15</v>
@@ -5879,10 +5896,10 @@
         <v>400</v>
       </c>
       <c r="G144">
-        <v>12.849600000000001</v>
+        <v>12.3</v>
       </c>
       <c r="H144">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="145" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
@@ -5933,16 +5950,16 @@
     </row>
     <row r="147" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A147" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="B147" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C147" t="s">
-        <v>555</v>
+        <v>300</v>
       </c>
       <c r="D147" t="s">
-        <v>332</v>
+        <v>301</v>
       </c>
       <c r="E147" t="s">
         <v>15</v>
@@ -5951,10 +5968,10 @@
         <v>400</v>
       </c>
       <c r="G147">
-        <v>12.849600000000001</v>
+        <v>12.3</v>
       </c>
       <c r="H147">
-        <v>15</v>
+        <v>6</v>
       </c>
     </row>
     <row r="148" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
@@ -5980,7 +5997,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="149" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A149" t="s">
         <v>9</v>
       </c>
@@ -6034,10 +6051,10 @@
         <v>9</v>
       </c>
       <c r="C151" t="s">
-        <v>424</v>
+        <v>303</v>
       </c>
       <c r="D151" t="s">
-        <v>31</v>
+        <v>304</v>
       </c>
       <c r="E151" t="s">
         <v>15</v>
@@ -6049,7 +6066,7 @@
         <v>12.3</v>
       </c>
       <c r="H151">
-        <v>9</v>
+        <v>6</v>
       </c>
     </row>
     <row r="152" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
@@ -6132,10 +6149,10 @@
         <v>9</v>
       </c>
       <c r="C155" t="s">
-        <v>288</v>
+        <v>306</v>
       </c>
       <c r="D155" t="s">
-        <v>289</v>
+        <v>307</v>
       </c>
       <c r="E155" t="s">
         <v>15</v>
@@ -6175,16 +6192,16 @@
     </row>
     <row r="157" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A157" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="B157" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C157" t="s">
-        <v>160</v>
+        <v>316</v>
       </c>
       <c r="D157" t="s">
-        <v>621</v>
+        <v>64</v>
       </c>
       <c r="E157" t="s">
         <v>15</v>
@@ -6193,10 +6210,10 @@
         <v>400</v>
       </c>
       <c r="G157">
-        <v>12.849600000000001</v>
+        <v>12.3</v>
       </c>
       <c r="H157">
-        <v>18</v>
+        <v>6</v>
       </c>
     </row>
     <row r="158" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
@@ -6343,7 +6360,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="164" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="164" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A164" t="s">
         <v>13</v>
       </c>
@@ -6403,10 +6420,10 @@
         <v>9</v>
       </c>
       <c r="C166" t="s">
-        <v>333</v>
+        <v>319</v>
       </c>
       <c r="D166" t="s">
-        <v>334</v>
+        <v>129</v>
       </c>
       <c r="E166" t="s">
         <v>15</v>
@@ -6418,7 +6435,7 @@
         <v>12.3</v>
       </c>
       <c r="H166">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="167" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
@@ -6455,10 +6472,10 @@
         <v>13</v>
       </c>
       <c r="C168" t="s">
-        <v>31</v>
+        <v>322</v>
       </c>
       <c r="D168" t="s">
-        <v>576</v>
+        <v>323</v>
       </c>
       <c r="E168" t="s">
         <v>15</v>
@@ -6470,7 +6487,7 @@
         <v>12.849600000000001</v>
       </c>
       <c r="H168">
-        <v>16</v>
+        <v>7</v>
       </c>
     </row>
     <row r="169" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
@@ -6498,16 +6515,16 @@
     </row>
     <row r="170" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A170" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="B170" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C170" t="s">
-        <v>601</v>
+        <v>324</v>
       </c>
       <c r="D170" t="s">
-        <v>290</v>
+        <v>325</v>
       </c>
       <c r="E170" t="s">
         <v>15</v>
@@ -6516,10 +6533,10 @@
         <v>400</v>
       </c>
       <c r="G170">
-        <v>12.849600000000001</v>
+        <v>12.3</v>
       </c>
       <c r="H170">
-        <v>17</v>
+        <v>7</v>
       </c>
     </row>
     <row r="171" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
@@ -6602,10 +6619,10 @@
         <v>9</v>
       </c>
       <c r="C174" t="s">
-        <v>459</v>
+        <v>327</v>
       </c>
       <c r="D174" t="s">
-        <v>102</v>
+        <v>328</v>
       </c>
       <c r="E174" t="s">
         <v>15</v>
@@ -6617,7 +6634,7 @@
         <v>12.3</v>
       </c>
       <c r="H174">
-        <v>10</v>
+        <v>7</v>
       </c>
     </row>
     <row r="175" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
@@ -6700,10 +6717,10 @@
         <v>9</v>
       </c>
       <c r="C178" t="s">
-        <v>381</v>
+        <v>330</v>
       </c>
       <c r="D178" t="s">
-        <v>382</v>
+        <v>331</v>
       </c>
       <c r="E178" t="s">
         <v>15</v>
@@ -6715,7 +6732,7 @@
         <v>12.3</v>
       </c>
       <c r="H178">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="179" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
@@ -6743,16 +6760,16 @@
     </row>
     <row r="180" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A180" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="B180" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C180" t="s">
-        <v>210</v>
+        <v>333</v>
       </c>
       <c r="D180" t="s">
-        <v>641</v>
+        <v>334</v>
       </c>
       <c r="E180" t="s">
         <v>15</v>
@@ -6761,10 +6778,10 @@
         <v>400</v>
       </c>
       <c r="G180">
-        <v>12.849600000000001</v>
+        <v>12.3</v>
       </c>
       <c r="H180">
-        <v>19</v>
+        <v>7</v>
       </c>
     </row>
     <row r="181" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
@@ -6934,7 +6951,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="188" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="188" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A188" t="s">
         <v>9</v>
       </c>
@@ -6988,10 +7005,10 @@
         <v>9</v>
       </c>
       <c r="C190" t="s">
-        <v>291</v>
+        <v>336</v>
       </c>
       <c r="D190" t="s">
-        <v>292</v>
+        <v>337</v>
       </c>
       <c r="E190" t="s">
         <v>15</v>
@@ -7003,7 +7020,7 @@
         <v>12.3</v>
       </c>
       <c r="H190">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="191" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
@@ -7034,16 +7051,16 @@
     </row>
     <row r="192" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A192" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="B192" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C192" t="s">
-        <v>102</v>
+        <v>339</v>
       </c>
       <c r="D192" t="s">
-        <v>557</v>
+        <v>340</v>
       </c>
       <c r="E192" t="s">
         <v>15</v>
@@ -7052,10 +7069,10 @@
         <v>400</v>
       </c>
       <c r="G192">
-        <v>12.849600000000001</v>
+        <v>12.3</v>
       </c>
       <c r="H192">
-        <v>15</v>
+        <v>7</v>
       </c>
     </row>
     <row r="193" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
@@ -7083,16 +7100,16 @@
     </row>
     <row r="194" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A194" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="B194" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C194" t="s">
-        <v>623</v>
+        <v>342</v>
       </c>
       <c r="D194" t="s">
-        <v>383</v>
+        <v>343</v>
       </c>
       <c r="E194" t="s">
         <v>15</v>
@@ -7101,10 +7118,10 @@
         <v>400</v>
       </c>
       <c r="G194">
-        <v>12.849600000000001</v>
+        <v>12.3</v>
       </c>
       <c r="H194">
-        <v>18</v>
+        <v>7</v>
       </c>
     </row>
     <row r="195" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
@@ -7210,10 +7227,10 @@
         <v>9</v>
       </c>
       <c r="C199" t="s">
-        <v>427</v>
+        <v>345</v>
       </c>
       <c r="D199" t="s">
-        <v>163</v>
+        <v>346</v>
       </c>
       <c r="E199" t="s">
         <v>15</v>
@@ -7225,7 +7242,7 @@
         <v>12.3</v>
       </c>
       <c r="H199">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="200" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
@@ -7308,10 +7325,10 @@
         <v>9</v>
       </c>
       <c r="C203" t="s">
-        <v>336</v>
+        <v>348</v>
       </c>
       <c r="D203" t="s">
-        <v>337</v>
+        <v>349</v>
       </c>
       <c r="E203" t="s">
         <v>15</v>
@@ -7351,16 +7368,16 @@
     </row>
     <row r="205" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A205" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="B205" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C205" t="s">
-        <v>251</v>
+        <v>351</v>
       </c>
       <c r="D205" t="s">
-        <v>578</v>
+        <v>352</v>
       </c>
       <c r="E205" t="s">
         <v>15</v>
@@ -7369,13 +7386,13 @@
         <v>400</v>
       </c>
       <c r="G205">
-        <v>12.849600000000001</v>
+        <v>12.3</v>
       </c>
       <c r="H205">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="206" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="206" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A206" t="s">
         <v>13</v>
       </c>
@@ -7579,10 +7596,10 @@
         <v>9</v>
       </c>
       <c r="C214" t="s">
-        <v>384</v>
+        <v>355</v>
       </c>
       <c r="D214" t="s">
-        <v>385</v>
+        <v>176</v>
       </c>
       <c r="E214" t="s">
         <v>15</v>
@@ -7594,7 +7611,7 @@
         <v>12.3</v>
       </c>
       <c r="H214">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="215" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
@@ -7631,10 +7648,10 @@
         <v>13</v>
       </c>
       <c r="C216" t="s">
-        <v>163</v>
+        <v>176</v>
       </c>
       <c r="D216" t="s">
-        <v>164</v>
+        <v>356</v>
       </c>
       <c r="E216" t="s">
         <v>15</v>
@@ -7646,7 +7663,7 @@
         <v>12.849600000000001</v>
       </c>
       <c r="H216">
-        <v>3</v>
+        <v>7</v>
       </c>
     </row>
     <row r="217" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
@@ -7697,16 +7714,16 @@
     </row>
     <row r="219" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A219" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="B219" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C219" t="s">
-        <v>603</v>
+        <v>261</v>
       </c>
       <c r="D219" t="s">
-        <v>338</v>
+        <v>262</v>
       </c>
       <c r="E219" t="s">
         <v>15</v>
@@ -7715,10 +7732,10 @@
         <v>400</v>
       </c>
       <c r="G219">
-        <v>12.849600000000001</v>
+        <v>12.3</v>
       </c>
       <c r="H219">
-        <v>17</v>
+        <v>7</v>
       </c>
     </row>
     <row r="220" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
@@ -7824,10 +7841,10 @@
         <v>9</v>
       </c>
       <c r="C224" t="s">
-        <v>462</v>
+        <v>358</v>
       </c>
       <c r="D224" t="s">
-        <v>213</v>
+        <v>359</v>
       </c>
       <c r="E224" t="s">
         <v>15</v>
@@ -7839,7 +7856,7 @@
         <v>12.3</v>
       </c>
       <c r="H224">
-        <v>10</v>
+        <v>7</v>
       </c>
     </row>
     <row r="225" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
@@ -7922,10 +7939,10 @@
         <v>9</v>
       </c>
       <c r="C228" t="s">
-        <v>294</v>
+        <v>361</v>
       </c>
       <c r="D228" t="s">
-        <v>295</v>
+        <v>362</v>
       </c>
       <c r="E228" t="s">
         <v>15</v>
@@ -7937,7 +7954,7 @@
         <v>12.3</v>
       </c>
       <c r="H228">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="229" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
@@ -7965,16 +7982,16 @@
     </row>
     <row r="230" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A230" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="B230" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C230" t="s">
-        <v>36</v>
+        <v>364</v>
       </c>
       <c r="D230" t="s">
-        <v>559</v>
+        <v>365</v>
       </c>
       <c r="E230" t="s">
         <v>15</v>
@@ -7983,13 +8000,13 @@
         <v>400</v>
       </c>
       <c r="G230">
-        <v>12.849600000000001</v>
+        <v>12.3</v>
       </c>
       <c r="H230">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="231" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="231" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A231" t="s">
         <v>9</v>
       </c>
@@ -8164,10 +8181,10 @@
         <v>9</v>
       </c>
       <c r="C238" t="s">
-        <v>339</v>
+        <v>368</v>
       </c>
       <c r="D238" t="s">
-        <v>340</v>
+        <v>369</v>
       </c>
       <c r="E238" t="s">
         <v>15</v>
@@ -8210,16 +8227,16 @@
     </row>
     <row r="240" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A240" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="B240" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C240" t="s">
-        <v>213</v>
+        <v>372</v>
       </c>
       <c r="D240" t="s">
-        <v>214</v>
+        <v>373</v>
       </c>
       <c r="E240" t="s">
         <v>15</v>
@@ -8228,10 +8245,10 @@
         <v>400</v>
       </c>
       <c r="G240">
-        <v>12.849600000000001</v>
+        <v>12.3</v>
       </c>
       <c r="H240">
-        <v>4</v>
+        <v>8</v>
       </c>
     </row>
     <row r="241" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
@@ -8282,16 +8299,16 @@
     </row>
     <row r="243" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A243" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="B243" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C243" t="s">
-        <v>580</v>
+        <v>375</v>
       </c>
       <c r="D243" t="s">
-        <v>296</v>
+        <v>376</v>
       </c>
       <c r="E243" t="s">
         <v>15</v>
@@ -8300,10 +8317,10 @@
         <v>400</v>
       </c>
       <c r="G243">
-        <v>12.849600000000001</v>
+        <v>12.3</v>
       </c>
       <c r="H243">
-        <v>16</v>
+        <v>8</v>
       </c>
     </row>
     <row r="244" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
@@ -8329,7 +8346,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="245" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="245" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A245" t="s">
         <v>13</v>
       </c>
@@ -8389,10 +8406,10 @@
         <v>9</v>
       </c>
       <c r="C247" t="s">
-        <v>430</v>
+        <v>378</v>
       </c>
       <c r="D247" t="s">
-        <v>38</v>
+        <v>379</v>
       </c>
       <c r="E247" t="s">
         <v>15</v>
@@ -8404,7 +8421,7 @@
         <v>12.3</v>
       </c>
       <c r="H247">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="248" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
@@ -8487,10 +8504,10 @@
         <v>9</v>
       </c>
       <c r="C251" t="s">
-        <v>387</v>
+        <v>381</v>
       </c>
       <c r="D251" t="s">
-        <v>388</v>
+        <v>382</v>
       </c>
       <c r="E251" t="s">
         <v>15</v>
@@ -8530,16 +8547,16 @@
     </row>
     <row r="253" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A253" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="B253" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C253" t="s">
-        <v>105</v>
+        <v>384</v>
       </c>
       <c r="D253" t="s">
-        <v>625</v>
+        <v>385</v>
       </c>
       <c r="E253" t="s">
         <v>15</v>
@@ -8548,10 +8565,10 @@
         <v>400</v>
       </c>
       <c r="G253">
-        <v>12.849600000000001</v>
+        <v>12.3</v>
       </c>
       <c r="H253">
-        <v>18</v>
+        <v>8</v>
       </c>
     </row>
     <row r="254" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
@@ -8755,10 +8772,10 @@
         <v>9</v>
       </c>
       <c r="C262" t="s">
-        <v>297</v>
+        <v>387</v>
       </c>
       <c r="D262" t="s">
-        <v>298</v>
+        <v>388</v>
       </c>
       <c r="E262" t="s">
         <v>15</v>
@@ -8770,7 +8787,7 @@
         <v>12.3</v>
       </c>
       <c r="H262">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="263" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
@@ -8801,16 +8818,16 @@
     </row>
     <row r="264" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A264" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="B264" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C264" t="s">
-        <v>38</v>
+        <v>390</v>
       </c>
       <c r="D264" t="s">
-        <v>561</v>
+        <v>391</v>
       </c>
       <c r="E264" t="s">
         <v>15</v>
@@ -8819,10 +8836,10 @@
         <v>400</v>
       </c>
       <c r="G264">
-        <v>12.849600000000001</v>
+        <v>12.3</v>
       </c>
       <c r="H264">
-        <v>15</v>
+        <v>8</v>
       </c>
     </row>
     <row r="265" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
@@ -8850,16 +8867,16 @@
     </row>
     <row r="266" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A266" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="B266" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C266" t="s">
-        <v>605</v>
+        <v>393</v>
       </c>
       <c r="D266" t="s">
-        <v>389</v>
+        <v>394</v>
       </c>
       <c r="E266" t="s">
         <v>15</v>
@@ -8868,10 +8885,10 @@
         <v>400</v>
       </c>
       <c r="G266">
-        <v>12.849600000000001</v>
+        <v>12.3</v>
       </c>
       <c r="H266">
-        <v>17</v>
+        <v>8</v>
       </c>
     </row>
     <row r="267" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
@@ -8897,7 +8914,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="268" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="268" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A268" t="s">
         <v>9</v>
       </c>
@@ -8951,10 +8968,10 @@
         <v>9</v>
       </c>
       <c r="C270" t="s">
-        <v>465</v>
+        <v>396</v>
       </c>
       <c r="D270" t="s">
-        <v>40</v>
+        <v>397</v>
       </c>
       <c r="E270" t="s">
         <v>15</v>
@@ -8966,7 +8983,7 @@
         <v>12.3</v>
       </c>
       <c r="H270">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="271" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
@@ -9049,10 +9066,10 @@
         <v>9</v>
       </c>
       <c r="C274" t="s">
-        <v>342</v>
+        <v>399</v>
       </c>
       <c r="D274" t="s">
-        <v>343</v>
+        <v>400</v>
       </c>
       <c r="E274" t="s">
         <v>15</v>
@@ -9064,7 +9081,7 @@
         <v>12.3</v>
       </c>
       <c r="H274">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="275" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
@@ -9098,10 +9115,10 @@
         <v>13</v>
       </c>
       <c r="C276" t="s">
-        <v>167</v>
+        <v>403</v>
       </c>
       <c r="D276" t="s">
-        <v>643</v>
+        <v>404</v>
       </c>
       <c r="E276" t="s">
         <v>15</v>
@@ -9113,7 +9130,7 @@
         <v>12.849600000000001</v>
       </c>
       <c r="H276">
-        <v>19</v>
+        <v>8</v>
       </c>
     </row>
     <row r="277" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
@@ -9283,7 +9300,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="284" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="284" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A284" t="s">
         <v>13</v>
       </c>
@@ -9343,10 +9360,10 @@
         <v>9</v>
       </c>
       <c r="C286" t="s">
-        <v>390</v>
+        <v>310</v>
       </c>
       <c r="D286" t="s">
-        <v>391</v>
+        <v>311</v>
       </c>
       <c r="E286" t="s">
         <v>15</v>
@@ -9389,16 +9406,16 @@
     </row>
     <row r="288" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A288" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="B288" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C288" t="s">
-        <v>40</v>
+        <v>406</v>
       </c>
       <c r="D288" t="s">
-        <v>582</v>
+        <v>407</v>
       </c>
       <c r="E288" t="s">
         <v>15</v>
@@ -9407,10 +9424,10 @@
         <v>400</v>
       </c>
       <c r="G288">
-        <v>12.849600000000001</v>
+        <v>12.3</v>
       </c>
       <c r="H288">
-        <v>16</v>
+        <v>8</v>
       </c>
     </row>
     <row r="289" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
@@ -9438,16 +9455,16 @@
     </row>
     <row r="290" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A290" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="B290" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C290" t="s">
-        <v>627</v>
+        <v>409</v>
       </c>
       <c r="D290" t="s">
-        <v>344</v>
+        <v>410</v>
       </c>
       <c r="E290" t="s">
         <v>15</v>
@@ -9456,10 +9473,10 @@
         <v>400</v>
       </c>
       <c r="G290">
-        <v>12.849600000000001</v>
+        <v>12.3</v>
       </c>
       <c r="H290">
-        <v>18</v>
+        <v>8</v>
       </c>
     </row>
     <row r="291" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
@@ -9542,10 +9559,10 @@
         <v>9</v>
       </c>
       <c r="C294" t="s">
-        <v>433</v>
+        <v>411</v>
       </c>
       <c r="D294" t="s">
-        <v>108</v>
+        <v>412</v>
       </c>
       <c r="E294" t="s">
         <v>15</v>
@@ -9557,7 +9574,7 @@
         <v>12.3</v>
       </c>
       <c r="H294">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="295" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
@@ -9640,10 +9657,10 @@
         <v>9</v>
       </c>
       <c r="C298" t="s">
-        <v>300</v>
+        <v>415</v>
       </c>
       <c r="D298" t="s">
-        <v>301</v>
+        <v>66</v>
       </c>
       <c r="E298" t="s">
         <v>15</v>
@@ -9655,7 +9672,7 @@
         <v>12.3</v>
       </c>
       <c r="H298">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="299" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
@@ -9683,16 +9700,16 @@
     </row>
     <row r="300" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A300" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="B300" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C300" t="s">
-        <v>217</v>
+        <v>421</v>
       </c>
       <c r="D300" t="s">
-        <v>563</v>
+        <v>206</v>
       </c>
       <c r="E300" t="s">
         <v>15</v>
@@ -9701,10 +9718,10 @@
         <v>400</v>
       </c>
       <c r="G300">
-        <v>12.849600000000001</v>
+        <v>12.3</v>
       </c>
       <c r="H300">
-        <v>15</v>
+        <v>9</v>
       </c>
     </row>
     <row r="301" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
@@ -9874,7 +9891,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="308" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="308" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A308" t="s">
         <v>9</v>
       </c>
@@ -9928,10 +9945,10 @@
         <v>9</v>
       </c>
       <c r="C310" t="s">
-        <v>345</v>
+        <v>424</v>
       </c>
       <c r="D310" t="s">
-        <v>346</v>
+        <v>31</v>
       </c>
       <c r="E310" t="s">
         <v>15</v>
@@ -9943,7 +9960,7 @@
         <v>12.3</v>
       </c>
       <c r="H310">
-        <v>7</v>
+        <v>9</v>
       </c>
     </row>
     <row r="311" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
@@ -9974,16 +9991,16 @@
     </row>
     <row r="312" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A312" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="B312" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C312" t="s">
-        <v>108</v>
+        <v>427</v>
       </c>
       <c r="D312" t="s">
-        <v>607</v>
+        <v>163</v>
       </c>
       <c r="E312" t="s">
         <v>15</v>
@@ -9992,10 +10009,10 @@
         <v>400</v>
       </c>
       <c r="G312">
-        <v>12.849600000000001</v>
+        <v>12.3</v>
       </c>
       <c r="H312">
-        <v>17</v>
+        <v>9</v>
       </c>
     </row>
     <row r="313" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
@@ -10023,16 +10040,16 @@
     </row>
     <row r="314" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A314" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="B314" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C314" t="s">
-        <v>645</v>
+        <v>430</v>
       </c>
       <c r="D314" t="s">
-        <v>302</v>
+        <v>38</v>
       </c>
       <c r="E314" t="s">
         <v>15</v>
@@ -10041,10 +10058,10 @@
         <v>400</v>
       </c>
       <c r="G314">
-        <v>12.849600000000001</v>
+        <v>12.3</v>
       </c>
       <c r="H314">
-        <v>19</v>
+        <v>9</v>
       </c>
     </row>
     <row r="315" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
@@ -10127,10 +10144,10 @@
         <v>9</v>
       </c>
       <c r="C318" t="s">
-        <v>468</v>
+        <v>433</v>
       </c>
       <c r="D318" t="s">
-        <v>170</v>
+        <v>108</v>
       </c>
       <c r="E318" t="s">
         <v>15</v>
@@ -10142,7 +10159,7 @@
         <v>12.3</v>
       </c>
       <c r="H318">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="319" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
@@ -10225,10 +10242,10 @@
         <v>9</v>
       </c>
       <c r="C322" t="s">
-        <v>393</v>
+        <v>436</v>
       </c>
       <c r="D322" t="s">
-        <v>394</v>
+        <v>220</v>
       </c>
       <c r="E322" t="s">
         <v>15</v>
@@ -10240,7 +10257,7 @@
         <v>12.3</v>
       </c>
       <c r="H322">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="323" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
@@ -10268,16 +10285,16 @@
     </row>
     <row r="324" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A324" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="B324" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C324" t="s">
-        <v>254</v>
+        <v>439</v>
       </c>
       <c r="D324" t="s">
-        <v>584</v>
+        <v>49</v>
       </c>
       <c r="E324" t="s">
         <v>15</v>
@@ -10286,13 +10303,13 @@
         <v>400</v>
       </c>
       <c r="G324">
-        <v>12.849600000000001</v>
+        <v>12.3</v>
       </c>
       <c r="H324">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="325" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="325" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A325" t="s">
         <v>13</v>
       </c>
@@ -10513,16 +10530,16 @@
     </row>
     <row r="334" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A334" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="B334" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="C334" t="s">
-        <v>303</v>
+        <v>49</v>
       </c>
       <c r="D334" t="s">
-        <v>304</v>
+        <v>440</v>
       </c>
       <c r="E334" t="s">
         <v>15</v>
@@ -10531,10 +10548,10 @@
         <v>400</v>
       </c>
       <c r="G334">
-        <v>12.3</v>
+        <v>12.849600000000001</v>
       </c>
       <c r="H334">
-        <v>6</v>
+        <v>9</v>
       </c>
     </row>
     <row r="335" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
@@ -10565,16 +10582,16 @@
     </row>
     <row r="336" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A336" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="B336" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C336" t="s">
-        <v>170</v>
+        <v>258</v>
       </c>
       <c r="D336" t="s">
-        <v>565</v>
+        <v>259</v>
       </c>
       <c r="E336" t="s">
         <v>15</v>
@@ -10583,10 +10600,10 @@
         <v>400</v>
       </c>
       <c r="G336">
-        <v>12.849600000000001</v>
+        <v>12.3</v>
       </c>
       <c r="H336">
-        <v>15</v>
+        <v>9</v>
       </c>
     </row>
     <row r="337" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
@@ -10614,16 +10631,16 @@
     </row>
     <row r="338" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A338" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="B338" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C338" t="s">
-        <v>629</v>
+        <v>442</v>
       </c>
       <c r="D338" t="s">
-        <v>395</v>
+        <v>443</v>
       </c>
       <c r="E338" t="s">
         <v>15</v>
@@ -10632,10 +10649,10 @@
         <v>400</v>
       </c>
       <c r="G338">
-        <v>12.849600000000001</v>
+        <v>12.3</v>
       </c>
       <c r="H338">
-        <v>18</v>
+        <v>9</v>
       </c>
     </row>
     <row r="339" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
@@ -10718,10 +10735,10 @@
         <v>9</v>
       </c>
       <c r="C342" t="s">
-        <v>436</v>
+        <v>313</v>
       </c>
       <c r="D342" t="s">
-        <v>220</v>
+        <v>314</v>
       </c>
       <c r="E342" t="s">
         <v>15</v>
@@ -10816,10 +10833,10 @@
         <v>9</v>
       </c>
       <c r="C346" t="s">
-        <v>348</v>
+        <v>447</v>
       </c>
       <c r="D346" t="s">
-        <v>349</v>
+        <v>231</v>
       </c>
       <c r="E346" t="s">
         <v>15</v>
@@ -10831,7 +10848,7 @@
         <v>12.3</v>
       </c>
       <c r="H346">
-        <v>7</v>
+        <v>9</v>
       </c>
     </row>
     <row r="347" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
@@ -10865,10 +10882,10 @@
         <v>13</v>
       </c>
       <c r="C348" t="s">
-        <v>45</v>
+        <v>448</v>
       </c>
       <c r="D348" t="s">
-        <v>609</v>
+        <v>449</v>
       </c>
       <c r="E348" t="s">
         <v>15</v>
@@ -10880,10 +10897,10 @@
         <v>12.849600000000001</v>
       </c>
       <c r="H348">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="349" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="349" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A349" t="s">
         <v>9</v>
       </c>
@@ -11127,10 +11144,10 @@
         <v>9</v>
       </c>
       <c r="C359" t="s">
-        <v>396</v>
+        <v>450</v>
       </c>
       <c r="D359" t="s">
-        <v>397</v>
+        <v>451</v>
       </c>
       <c r="E359" t="s">
         <v>15</v>
@@ -11142,7 +11159,7 @@
         <v>12.3</v>
       </c>
       <c r="H359">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="360" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
@@ -11173,16 +11190,16 @@
     </row>
     <row r="361" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A361" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="B361" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C361" t="s">
-        <v>220</v>
+        <v>456</v>
       </c>
       <c r="D361" t="s">
-        <v>586</v>
+        <v>29</v>
       </c>
       <c r="E361" t="s">
         <v>15</v>
@@ -11191,10 +11208,10 @@
         <v>400</v>
       </c>
       <c r="G361">
-        <v>12.849600000000001</v>
+        <v>12.3</v>
       </c>
       <c r="H361">
-        <v>16</v>
+        <v>10</v>
       </c>
     </row>
     <row r="362" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
@@ -11222,16 +11239,16 @@
     </row>
     <row r="363" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A363" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="B363" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C363" t="s">
-        <v>647</v>
+        <v>459</v>
       </c>
       <c r="D363" t="s">
-        <v>350</v>
+        <v>102</v>
       </c>
       <c r="E363" t="s">
         <v>15</v>
@@ -11240,10 +11257,10 @@
         <v>400</v>
       </c>
       <c r="G363">
-        <v>12.849600000000001</v>
+        <v>12.3</v>
       </c>
       <c r="H363">
-        <v>19</v>
+        <v>10</v>
       </c>
     </row>
     <row r="364" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
@@ -11269,7 +11286,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="365" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="365" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A365" t="s">
         <v>13</v>
       </c>
@@ -11329,10 +11346,10 @@
         <v>9</v>
       </c>
       <c r="C367" t="s">
-        <v>471</v>
+        <v>462</v>
       </c>
       <c r="D367" t="s">
-        <v>47</v>
+        <v>213</v>
       </c>
       <c r="E367" t="s">
         <v>15</v>
@@ -11496,10 +11513,10 @@
         <v>9</v>
       </c>
       <c r="C374" t="s">
-        <v>306</v>
+        <v>465</v>
       </c>
       <c r="D374" t="s">
-        <v>307</v>
+        <v>40</v>
       </c>
       <c r="E374" t="s">
         <v>15</v>
@@ -11511,7 +11528,7 @@
         <v>12.3</v>
       </c>
       <c r="H374">
-        <v>6</v>
+        <v>10</v>
       </c>
     </row>
     <row r="375" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
@@ -11539,16 +11556,16 @@
     </row>
     <row r="376" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A376" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="B376" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C376" t="s">
-        <v>111</v>
+        <v>468</v>
       </c>
       <c r="D376" t="s">
-        <v>654</v>
+        <v>170</v>
       </c>
       <c r="E376" t="s">
         <v>15</v>
@@ -11557,10 +11574,10 @@
         <v>400</v>
       </c>
       <c r="G376">
-        <v>12.849600000000001</v>
+        <v>12.3</v>
       </c>
       <c r="H376">
-        <v>20</v>
+        <v>10</v>
       </c>
     </row>
     <row r="377" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
@@ -11833,10 +11850,10 @@
         <v>9</v>
       </c>
       <c r="C388" t="s">
-        <v>351</v>
+        <v>471</v>
       </c>
       <c r="D388" t="s">
-        <v>352</v>
+        <v>47</v>
       </c>
       <c r="E388" t="s">
         <v>15</v>
@@ -11848,7 +11865,7 @@
         <v>12.3</v>
       </c>
       <c r="H388">
-        <v>7</v>
+        <v>10</v>
       </c>
     </row>
     <row r="389" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
@@ -11928,16 +11945,16 @@
     </row>
     <row r="392" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A392" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="B392" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C392" t="s">
-        <v>611</v>
+        <v>473</v>
       </c>
       <c r="D392" t="s">
-        <v>612</v>
+        <v>474</v>
       </c>
       <c r="E392" t="s">
         <v>15</v>
@@ -11946,10 +11963,10 @@
         <v>400</v>
       </c>
       <c r="G392">
-        <v>12.849600000000001</v>
+        <v>12.3</v>
       </c>
       <c r="H392">
-        <v>17</v>
+        <v>10</v>
       </c>
     </row>
     <row r="393" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
@@ -11998,7 +12015,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="395" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="395" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A395" t="s">
         <v>9</v>
       </c>
@@ -12052,10 +12069,10 @@
         <v>9</v>
       </c>
       <c r="C397" t="s">
-        <v>439</v>
+        <v>476</v>
       </c>
       <c r="D397" t="s">
-        <v>49</v>
+        <v>477</v>
       </c>
       <c r="E397" t="s">
         <v>15</v>
@@ -12067,7 +12084,7 @@
         <v>12.3</v>
       </c>
       <c r="H397">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="398" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
@@ -12142,7 +12159,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="401" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="401" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A401" t="s">
         <v>8</v>
       </c>
@@ -12219,10 +12236,10 @@
         <v>9</v>
       </c>
       <c r="C404" t="s">
-        <v>399</v>
+        <v>480</v>
       </c>
       <c r="D404" t="s">
-        <v>400</v>
+        <v>57</v>
       </c>
       <c r="E404" t="s">
         <v>15</v>
@@ -12234,21 +12251,21 @@
         <v>12.3</v>
       </c>
       <c r="H404">
-        <v>8</v>
+        <v>10</v>
       </c>
     </row>
     <row r="405" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A405" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="B405" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C405" t="s">
-        <v>173</v>
+        <v>483</v>
       </c>
       <c r="D405" t="s">
-        <v>588</v>
+        <v>182</v>
       </c>
       <c r="E405" t="s">
         <v>15</v>
@@ -12257,10 +12274,10 @@
         <v>400</v>
       </c>
       <c r="G405">
-        <v>12.849600000000001</v>
+        <v>12.3</v>
       </c>
       <c r="H405">
-        <v>16</v>
+        <v>10</v>
       </c>
     </row>
     <row r="406" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
@@ -12481,16 +12498,16 @@
     </row>
     <row r="415" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A415" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="B415" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="C415" t="s">
-        <v>473</v>
+        <v>486</v>
       </c>
       <c r="D415" t="s">
-        <v>474</v>
+        <v>487</v>
       </c>
       <c r="E415" t="s">
         <v>15</v>
@@ -12499,7 +12516,7 @@
         <v>400</v>
       </c>
       <c r="G415">
-        <v>12.3</v>
+        <v>12.849600000000001</v>
       </c>
       <c r="H415">
         <v>10</v>
@@ -12539,10 +12556,10 @@
         <v>13</v>
       </c>
       <c r="C417" t="s">
-        <v>49</v>
+        <v>488</v>
       </c>
       <c r="D417" t="s">
-        <v>440</v>
+        <v>489</v>
       </c>
       <c r="E417" t="s">
         <v>15</v>
@@ -12554,10 +12571,10 @@
         <v>12.849600000000001</v>
       </c>
       <c r="H417">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="418" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="418" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A418" t="s">
         <v>8</v>
       </c>
@@ -12605,16 +12622,16 @@
     </row>
     <row r="420" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A420" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="B420" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C420" t="s">
-        <v>631</v>
+        <v>498</v>
       </c>
       <c r="D420" t="s">
-        <v>632</v>
+        <v>114</v>
       </c>
       <c r="E420" t="s">
         <v>15</v>
@@ -12623,10 +12640,10 @@
         <v>400</v>
       </c>
       <c r="G420">
-        <v>12.849600000000001</v>
+        <v>12.3</v>
       </c>
       <c r="H420">
-        <v>18</v>
+        <v>11</v>
       </c>
     </row>
     <row r="421" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
@@ -12778,10 +12795,10 @@
         <v>9</v>
       </c>
       <c r="C427" t="s">
-        <v>498</v>
+        <v>501</v>
       </c>
       <c r="D427" t="s">
-        <v>114</v>
+        <v>55</v>
       </c>
       <c r="E427" t="s">
         <v>15</v>
@@ -12899,10 +12916,10 @@
         <v>9</v>
       </c>
       <c r="C432" t="s">
-        <v>515</v>
+        <v>504</v>
       </c>
       <c r="D432" t="s">
-        <v>516</v>
+        <v>120</v>
       </c>
       <c r="E432" t="s">
         <v>15</v>
@@ -12914,7 +12931,7 @@
         <v>12.3</v>
       </c>
       <c r="H432">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="433" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
@@ -12965,16 +12982,16 @@
     </row>
     <row r="435" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A435" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="B435" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C435" t="s">
-        <v>223</v>
+        <v>506</v>
       </c>
       <c r="D435" t="s">
-        <v>614</v>
+        <v>507</v>
       </c>
       <c r="E435" t="s">
         <v>15</v>
@@ -12983,10 +13000,10 @@
         <v>400</v>
       </c>
       <c r="G435">
-        <v>12.849600000000001</v>
+        <v>12.3</v>
       </c>
       <c r="H435">
-        <v>19</v>
+        <v>11</v>
       </c>
     </row>
     <row r="436" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
@@ -13110,7 +13127,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="441" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="441" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A441" t="s">
         <v>13</v>
       </c>
@@ -13236,16 +13253,16 @@
     </row>
     <row r="446" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A446" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="B446" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="C446" t="s">
-        <v>258</v>
+        <v>508</v>
       </c>
       <c r="D446" t="s">
-        <v>259</v>
+        <v>509</v>
       </c>
       <c r="E446" t="s">
         <v>15</v>
@@ -13254,10 +13271,10 @@
         <v>400</v>
       </c>
       <c r="G446">
-        <v>12.3</v>
+        <v>12.849600000000001</v>
       </c>
       <c r="H446">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="447" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
@@ -13285,16 +13302,16 @@
     </row>
     <row r="448" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A448" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="B448" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C448" t="s">
-        <v>114</v>
+        <v>515</v>
       </c>
       <c r="D448" t="s">
-        <v>589</v>
+        <v>516</v>
       </c>
       <c r="E448" t="s">
         <v>15</v>
@@ -13303,10 +13320,10 @@
         <v>400</v>
       </c>
       <c r="G448">
-        <v>12.849600000000001</v>
+        <v>12.3</v>
       </c>
       <c r="H448">
-        <v>16</v>
+        <v>12</v>
       </c>
     </row>
     <row r="449" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
@@ -13357,16 +13374,16 @@
     </row>
     <row r="451" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A451" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="B451" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C451" t="s">
-        <v>403</v>
+        <v>519</v>
       </c>
       <c r="D451" t="s">
-        <v>404</v>
+        <v>520</v>
       </c>
       <c r="E451" t="s">
         <v>15</v>
@@ -13375,10 +13392,10 @@
         <v>400</v>
       </c>
       <c r="G451">
-        <v>12.849600000000001</v>
+        <v>12.3</v>
       </c>
       <c r="H451">
-        <v>8</v>
+        <v>12</v>
       </c>
     </row>
     <row r="452" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
@@ -13501,16 +13518,16 @@
     </row>
     <row r="457" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A457" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="B457" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="C457" t="s">
-        <v>355</v>
+        <v>523</v>
       </c>
       <c r="D457" t="s">
-        <v>176</v>
+        <v>524</v>
       </c>
       <c r="E457" t="s">
         <v>15</v>
@@ -13519,10 +13536,10 @@
         <v>400</v>
       </c>
       <c r="G457">
-        <v>12.3</v>
+        <v>12.849600000000001</v>
       </c>
       <c r="H457">
-        <v>7</v>
+        <v>12</v>
       </c>
     </row>
     <row r="458" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
@@ -13645,16 +13662,16 @@
     </row>
     <row r="463" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A463" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="B463" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="C463" t="s">
-        <v>476</v>
+        <v>541</v>
       </c>
       <c r="D463" t="s">
-        <v>477</v>
+        <v>542</v>
       </c>
       <c r="E463" t="s">
         <v>15</v>
@@ -13663,10 +13680,10 @@
         <v>400</v>
       </c>
       <c r="G463">
-        <v>12.3</v>
+        <v>12.849600000000001</v>
       </c>
       <c r="H463">
-        <v>10</v>
+        <v>13</v>
       </c>
     </row>
     <row r="464" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
@@ -13700,10 +13717,10 @@
         <v>13</v>
       </c>
       <c r="C465" t="s">
-        <v>53</v>
+        <v>543</v>
       </c>
       <c r="D465" t="s">
-        <v>567</v>
+        <v>544</v>
       </c>
       <c r="E465" t="s">
         <v>15</v>
@@ -13715,10 +13732,10 @@
         <v>12.849600000000001</v>
       </c>
       <c r="H465">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="466" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="466" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A466" t="s">
         <v>9</v>
       </c>
@@ -13982,16 +13999,16 @@
     </row>
     <row r="477" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A477" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="B477" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="C477" t="s">
-        <v>310</v>
+        <v>546</v>
       </c>
       <c r="D477" t="s">
-        <v>311</v>
+        <v>547</v>
       </c>
       <c r="E477" t="s">
         <v>15</v>
@@ -14000,10 +14017,10 @@
         <v>400</v>
       </c>
       <c r="G477">
-        <v>12.3</v>
+        <v>12.849600000000001</v>
       </c>
       <c r="H477">
-        <v>8</v>
+        <v>14</v>
       </c>
     </row>
     <row r="478" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
@@ -14014,10 +14031,10 @@
         <v>13</v>
       </c>
       <c r="C478" t="s">
-        <v>176</v>
+        <v>550</v>
       </c>
       <c r="D478" t="s">
-        <v>356</v>
+        <v>63</v>
       </c>
       <c r="E478" t="s">
         <v>15</v>
@@ -14029,7 +14046,7 @@
         <v>12.849600000000001</v>
       </c>
       <c r="H478">
-        <v>7</v>
+        <v>14</v>
       </c>
     </row>
     <row r="479" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
@@ -14086,10 +14103,10 @@
         <v>13</v>
       </c>
       <c r="C481" t="s">
-        <v>546</v>
+        <v>154</v>
       </c>
       <c r="D481" t="s">
-        <v>547</v>
+        <v>552</v>
       </c>
       <c r="E481" t="s">
         <v>15</v>
@@ -14101,7 +14118,7 @@
         <v>12.849600000000001</v>
       </c>
       <c r="H481">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="482" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
@@ -14173,7 +14190,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="485" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="485" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A485" t="s">
         <v>13</v>
       </c>
@@ -14227,16 +14244,16 @@
     </row>
     <row r="487" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A487" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="B487" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="C487" t="s">
-        <v>501</v>
+        <v>555</v>
       </c>
       <c r="D487" t="s">
-        <v>55</v>
+        <v>332</v>
       </c>
       <c r="E487" t="s">
         <v>15</v>
@@ -14245,10 +14262,10 @@
         <v>400</v>
       </c>
       <c r="G487">
-        <v>12.3</v>
+        <v>12.849600000000001</v>
       </c>
       <c r="H487">
-        <v>11</v>
+        <v>15</v>
       </c>
     </row>
     <row r="488" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
@@ -14348,16 +14365,16 @@
     </row>
     <row r="492" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A492" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="B492" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="C492" t="s">
-        <v>442</v>
+        <v>102</v>
       </c>
       <c r="D492" t="s">
-        <v>443</v>
+        <v>557</v>
       </c>
       <c r="E492" t="s">
         <v>15</v>
@@ -14366,10 +14383,10 @@
         <v>400</v>
       </c>
       <c r="G492">
-        <v>12.3</v>
+        <v>12.849600000000001</v>
       </c>
       <c r="H492">
-        <v>9</v>
+        <v>15</v>
       </c>
     </row>
     <row r="493" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
@@ -14403,10 +14420,10 @@
         <v>13</v>
       </c>
       <c r="C494" t="s">
-        <v>117</v>
+        <v>36</v>
       </c>
       <c r="D494" t="s">
-        <v>615</v>
+        <v>559</v>
       </c>
       <c r="E494" t="s">
         <v>15</v>
@@ -14418,7 +14435,7 @@
         <v>12.849600000000001</v>
       </c>
       <c r="H494">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="495" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
@@ -14642,16 +14659,16 @@
     </row>
     <row r="504" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A504" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="B504" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="C504" t="s">
-        <v>261</v>
+        <v>38</v>
       </c>
       <c r="D504" t="s">
-        <v>262</v>
+        <v>561</v>
       </c>
       <c r="E504" t="s">
         <v>15</v>
@@ -14660,10 +14677,10 @@
         <v>400</v>
       </c>
       <c r="G504">
-        <v>12.3</v>
+        <v>12.849600000000001</v>
       </c>
       <c r="H504">
-        <v>7</v>
+        <v>15</v>
       </c>
     </row>
     <row r="505" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
@@ -14674,10 +14691,10 @@
         <v>13</v>
       </c>
       <c r="C505" t="s">
-        <v>55</v>
+        <v>217</v>
       </c>
       <c r="D505" t="s">
-        <v>569</v>
+        <v>563</v>
       </c>
       <c r="E505" t="s">
         <v>15</v>
@@ -14769,10 +14786,10 @@
         <v>13</v>
       </c>
       <c r="C509" t="s">
-        <v>634</v>
+        <v>170</v>
       </c>
       <c r="D509" t="s">
-        <v>444</v>
+        <v>565</v>
       </c>
       <c r="E509" t="s">
         <v>15</v>
@@ -14784,7 +14801,7 @@
         <v>12.849600000000001</v>
       </c>
       <c r="H509">
-        <v>18</v>
+        <v>15</v>
       </c>
     </row>
     <row r="510" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
@@ -14810,7 +14827,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="511" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="511" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A511" t="s">
         <v>13</v>
       </c>
@@ -14856,7 +14873,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="513" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="513" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A513" t="s">
         <v>9</v>
       </c>
@@ -14864,10 +14881,10 @@
         <v>13</v>
       </c>
       <c r="C513" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="D513" t="s">
-        <v>58</v>
+        <v>567</v>
       </c>
       <c r="E513" t="s">
         <v>15</v>
@@ -14879,7 +14896,7 @@
         <v>12.849600000000001</v>
       </c>
       <c r="H513">
-        <v>1</v>
+        <v>15</v>
       </c>
     </row>
     <row r="514" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
@@ -14907,16 +14924,16 @@
     </row>
     <row r="515" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A515" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="B515" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="C515" t="s">
-        <v>480</v>
+        <v>55</v>
       </c>
       <c r="D515" t="s">
-        <v>57</v>
+        <v>569</v>
       </c>
       <c r="E515" t="s">
         <v>15</v>
@@ -14925,10 +14942,10 @@
         <v>400</v>
       </c>
       <c r="G515">
-        <v>12.3</v>
+        <v>12.849600000000001</v>
       </c>
       <c r="H515">
-        <v>10</v>
+        <v>15</v>
       </c>
     </row>
     <row r="516" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
@@ -15005,16 +15022,16 @@
     </row>
     <row r="519" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A519" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="B519" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="C519" t="s">
-        <v>406</v>
+        <v>572</v>
       </c>
       <c r="D519" t="s">
-        <v>407</v>
+        <v>326</v>
       </c>
       <c r="E519" t="s">
         <v>15</v>
@@ -15023,10 +15040,10 @@
         <v>400</v>
       </c>
       <c r="G519">
-        <v>12.3</v>
+        <v>12.849600000000001</v>
       </c>
       <c r="H519">
-        <v>8</v>
+        <v>16</v>
       </c>
     </row>
     <row r="520" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
@@ -15060,10 +15077,10 @@
         <v>13</v>
       </c>
       <c r="C521" t="s">
-        <v>179</v>
+        <v>574</v>
       </c>
       <c r="D521" t="s">
-        <v>592</v>
+        <v>377</v>
       </c>
       <c r="E521" t="s">
         <v>15</v>
@@ -15322,16 +15339,16 @@
     </row>
     <row r="532" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A532" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="B532" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="C532" t="s">
-        <v>313</v>
+        <v>31</v>
       </c>
       <c r="D532" t="s">
-        <v>314</v>
+        <v>576</v>
       </c>
       <c r="E532" t="s">
         <v>15</v>
@@ -15340,13 +15357,13 @@
         <v>400</v>
       </c>
       <c r="G532">
-        <v>12.3</v>
+        <v>12.849600000000001</v>
       </c>
       <c r="H532">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="533" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="533" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A533" t="s">
         <v>13</v>
       </c>
@@ -15392,7 +15409,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="535" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="535" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A535" t="s">
         <v>13</v>
       </c>
@@ -15472,10 +15489,10 @@
         <v>13</v>
       </c>
       <c r="C538" t="s">
-        <v>617</v>
+        <v>251</v>
       </c>
       <c r="D538" t="s">
-        <v>408</v>
+        <v>578</v>
       </c>
       <c r="E538" t="s">
         <v>15</v>
@@ -15487,7 +15504,7 @@
         <v>12.849600000000001</v>
       </c>
       <c r="H538">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="539" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
@@ -15587,16 +15604,16 @@
     </row>
     <row r="543" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A543" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="B543" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="C543" t="s">
-        <v>504</v>
+        <v>580</v>
       </c>
       <c r="D543" t="s">
-        <v>120</v>
+        <v>296</v>
       </c>
       <c r="E543" t="s">
         <v>15</v>
@@ -15605,10 +15622,10 @@
         <v>400</v>
       </c>
       <c r="G543">
-        <v>12.3</v>
+        <v>12.849600000000001</v>
       </c>
       <c r="H543">
-        <v>11</v>
+        <v>16</v>
       </c>
     </row>
     <row r="544" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
@@ -15685,16 +15702,16 @@
     </row>
     <row r="547" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A547" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="B547" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="C547" t="s">
-        <v>358</v>
+        <v>40</v>
       </c>
       <c r="D547" t="s">
-        <v>359</v>
+        <v>582</v>
       </c>
       <c r="E547" t="s">
         <v>15</v>
@@ -15703,10 +15720,10 @@
         <v>400</v>
       </c>
       <c r="G547">
-        <v>12.3</v>
+        <v>12.849600000000001</v>
       </c>
       <c r="H547">
-        <v>7</v>
+        <v>16</v>
       </c>
     </row>
     <row r="548" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
@@ -15717,10 +15734,10 @@
         <v>13</v>
       </c>
       <c r="C548" t="s">
-        <v>228</v>
+        <v>254</v>
       </c>
       <c r="D548" t="s">
-        <v>651</v>
+        <v>584</v>
       </c>
       <c r="E548" t="s">
         <v>15</v>
@@ -15732,7 +15749,7 @@
         <v>12.849600000000001</v>
       </c>
       <c r="H548">
-        <v>19</v>
+        <v>16</v>
       </c>
     </row>
     <row r="549" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
@@ -15925,7 +15942,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="557" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="557" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A557" t="s">
         <v>9</v>
       </c>
@@ -15950,16 +15967,16 @@
     </row>
     <row r="558" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A558" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="B558" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="C558" t="s">
-        <v>409</v>
+        <v>220</v>
       </c>
       <c r="D558" t="s">
-        <v>410</v>
+        <v>586</v>
       </c>
       <c r="E558" t="s">
         <v>15</v>
@@ -15968,10 +15985,10 @@
         <v>400</v>
       </c>
       <c r="G558">
-        <v>12.3</v>
+        <v>12.849600000000001</v>
       </c>
       <c r="H558">
-        <v>8</v>
+        <v>16</v>
       </c>
     </row>
     <row r="559" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
@@ -16008,10 +16025,10 @@
         <v>13</v>
       </c>
       <c r="C560" t="s">
-        <v>120</v>
+        <v>173</v>
       </c>
       <c r="D560" t="s">
-        <v>121</v>
+        <v>588</v>
       </c>
       <c r="E560" t="s">
         <v>15</v>
@@ -16023,7 +16040,7 @@
         <v>12.849600000000001</v>
       </c>
       <c r="H560">
-        <v>2</v>
+        <v>16</v>
       </c>
     </row>
     <row r="561" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
@@ -16103,10 +16120,10 @@
         <v>13</v>
       </c>
       <c r="C564" t="s">
-        <v>594</v>
+        <v>114</v>
       </c>
       <c r="D564" t="s">
-        <v>360</v>
+        <v>589</v>
       </c>
       <c r="E564" t="s">
         <v>15</v>
@@ -16241,16 +16258,16 @@
     </row>
     <row r="570" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A570" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="B570" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="C570" t="s">
-        <v>483</v>
+        <v>179</v>
       </c>
       <c r="D570" t="s">
-        <v>182</v>
+        <v>592</v>
       </c>
       <c r="E570" t="s">
         <v>15</v>
@@ -16259,10 +16276,10 @@
         <v>400</v>
       </c>
       <c r="G570">
-        <v>12.3</v>
+        <v>12.849600000000001</v>
       </c>
       <c r="H570">
-        <v>10</v>
+        <v>16</v>
       </c>
     </row>
     <row r="571" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
@@ -16362,16 +16379,16 @@
     </row>
     <row r="575" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A575" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="B575" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="C575" t="s">
-        <v>519</v>
+        <v>594</v>
       </c>
       <c r="D575" t="s">
-        <v>520</v>
+        <v>360</v>
       </c>
       <c r="E575" t="s">
         <v>15</v>
@@ -16380,10 +16397,10 @@
         <v>400</v>
       </c>
       <c r="G575">
-        <v>12.3</v>
+        <v>12.849600000000001</v>
       </c>
       <c r="H575">
-        <v>12</v>
+        <v>16</v>
       </c>
     </row>
     <row r="576" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
@@ -16417,10 +16434,10 @@
         <v>13</v>
       </c>
       <c r="C577" t="s">
-        <v>315</v>
+        <v>247</v>
       </c>
       <c r="D577" t="s">
-        <v>636</v>
+        <v>597</v>
       </c>
       <c r="E577" t="s">
         <v>15</v>
@@ -16432,10 +16449,10 @@
         <v>12.849600000000001</v>
       </c>
       <c r="H577">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="578" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="578" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A578" t="s">
         <v>13</v>
       </c>
@@ -16610,16 +16627,16 @@
     </row>
     <row r="585" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A585" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="B585" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="C585" t="s">
-        <v>361</v>
+        <v>99</v>
       </c>
       <c r="D585" t="s">
-        <v>362</v>
+        <v>599</v>
       </c>
       <c r="E585" t="s">
         <v>15</v>
@@ -16628,10 +16645,10 @@
         <v>400</v>
       </c>
       <c r="G585">
-        <v>12.3</v>
+        <v>12.849600000000001</v>
       </c>
       <c r="H585">
-        <v>7</v>
+        <v>17</v>
       </c>
     </row>
     <row r="586" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
@@ -16714,10 +16731,10 @@
         <v>13</v>
       </c>
       <c r="C589" t="s">
-        <v>182</v>
+        <v>601</v>
       </c>
       <c r="D589" t="s">
-        <v>183</v>
+        <v>290</v>
       </c>
       <c r="E589" t="s">
         <v>15</v>
@@ -16729,7 +16746,7 @@
         <v>12.849600000000001</v>
       </c>
       <c r="H589">
-        <v>3</v>
+        <v>17</v>
       </c>
     </row>
     <row r="590" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
@@ -16763,10 +16780,10 @@
         <v>13</v>
       </c>
       <c r="C591" t="s">
-        <v>541</v>
+        <v>603</v>
       </c>
       <c r="D591" t="s">
-        <v>542</v>
+        <v>338</v>
       </c>
       <c r="E591" t="s">
         <v>15</v>
@@ -16778,7 +16795,7 @@
         <v>12.849600000000001</v>
       </c>
       <c r="H591">
-        <v>13</v>
+        <v>17</v>
       </c>
     </row>
     <row r="592" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
@@ -16878,16 +16895,16 @@
     </row>
     <row r="596" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A596" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="B596" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="C596" t="s">
-        <v>447</v>
+        <v>605</v>
       </c>
       <c r="D596" t="s">
-        <v>231</v>
+        <v>389</v>
       </c>
       <c r="E596" t="s">
         <v>15</v>
@@ -16896,10 +16913,10 @@
         <v>400</v>
       </c>
       <c r="G596">
-        <v>12.3</v>
+        <v>12.849600000000001</v>
       </c>
       <c r="H596">
-        <v>9</v>
+        <v>17</v>
       </c>
     </row>
     <row r="597" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
@@ -17045,16 +17062,16 @@
     </row>
     <row r="603" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A603" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="B603" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="C603" t="s">
-        <v>411</v>
+        <v>108</v>
       </c>
       <c r="D603" t="s">
-        <v>412</v>
+        <v>607</v>
       </c>
       <c r="E603" t="s">
         <v>15</v>
@@ -17063,10 +17080,10 @@
         <v>400</v>
       </c>
       <c r="G603">
-        <v>12.3</v>
+        <v>12.849600000000001</v>
       </c>
       <c r="H603">
-        <v>8</v>
+        <v>17</v>
       </c>
     </row>
     <row r="604" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
@@ -17092,7 +17109,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="605" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="605" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A605" t="s">
         <v>9</v>
       </c>
@@ -17123,10 +17140,10 @@
         <v>13</v>
       </c>
       <c r="C606" t="s">
-        <v>550</v>
+        <v>45</v>
       </c>
       <c r="D606" t="s">
-        <v>63</v>
+        <v>609</v>
       </c>
       <c r="E606" t="s">
         <v>15</v>
@@ -17138,7 +17155,7 @@
         <v>12.849600000000001</v>
       </c>
       <c r="H606">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="607" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
@@ -17264,16 +17281,16 @@
     </row>
     <row r="612" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A612" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="B612" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="C612" t="s">
-        <v>506</v>
+        <v>611</v>
       </c>
       <c r="D612" t="s">
-        <v>507</v>
+        <v>612</v>
       </c>
       <c r="E612" t="s">
         <v>15</v>
@@ -17282,10 +17299,10 @@
         <v>400</v>
       </c>
       <c r="G612">
-        <v>12.3</v>
+        <v>12.849600000000001</v>
       </c>
       <c r="H612">
-        <v>11</v>
+        <v>17</v>
       </c>
     </row>
     <row r="613" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
@@ -17342,10 +17359,10 @@
         <v>13</v>
       </c>
       <c r="C615" t="s">
-        <v>232</v>
+        <v>117</v>
       </c>
       <c r="D615" t="s">
-        <v>233</v>
+        <v>615</v>
       </c>
       <c r="E615" t="s">
         <v>15</v>
@@ -17357,7 +17374,7 @@
         <v>12.849600000000001</v>
       </c>
       <c r="H615">
-        <v>4</v>
+        <v>17</v>
       </c>
     </row>
     <row r="616" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
@@ -17368,10 +17385,10 @@
         <v>13</v>
       </c>
       <c r="C616" t="s">
-        <v>448</v>
+        <v>617</v>
       </c>
       <c r="D616" t="s">
-        <v>449</v>
+        <v>408</v>
       </c>
       <c r="E616" t="s">
         <v>15</v>
@@ -17383,7 +17400,7 @@
         <v>12.849600000000001</v>
       </c>
       <c r="H616">
-        <v>9</v>
+        <v>17</v>
       </c>
     </row>
     <row r="617" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
@@ -17409,7 +17426,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="618" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="618" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A618" t="s">
         <v>13</v>
       </c>
@@ -17463,16 +17480,16 @@
     </row>
     <row r="620" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A620" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="B620" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="C620" t="s">
-        <v>316</v>
+        <v>619</v>
       </c>
       <c r="D620" t="s">
-        <v>64</v>
+        <v>284</v>
       </c>
       <c r="E620" t="s">
         <v>15</v>
@@ -17481,10 +17498,10 @@
         <v>400</v>
       </c>
       <c r="G620">
-        <v>12.3</v>
+        <v>12.849600000000001</v>
       </c>
       <c r="H620">
-        <v>6</v>
+        <v>18</v>
       </c>
     </row>
     <row r="621" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
@@ -17607,16 +17624,16 @@
     </row>
     <row r="626" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A626" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="B626" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="C626" t="s">
-        <v>364</v>
+        <v>160</v>
       </c>
       <c r="D626" t="s">
-        <v>365</v>
+        <v>621</v>
       </c>
       <c r="E626" t="s">
         <v>15</v>
@@ -17625,10 +17642,10 @@
         <v>400</v>
       </c>
       <c r="G626">
-        <v>12.3</v>
+        <v>12.849600000000001</v>
       </c>
       <c r="H626">
-        <v>7</v>
+        <v>18</v>
       </c>
     </row>
     <row r="627" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
@@ -17662,10 +17679,10 @@
         <v>13</v>
       </c>
       <c r="C628" t="s">
-        <v>486</v>
+        <v>623</v>
       </c>
       <c r="D628" t="s">
-        <v>487</v>
+        <v>383</v>
       </c>
       <c r="E628" t="s">
         <v>15</v>
@@ -17677,7 +17694,7 @@
         <v>12.849600000000001</v>
       </c>
       <c r="H628">
-        <v>10</v>
+        <v>18</v>
       </c>
     </row>
     <row r="629" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
@@ -17826,16 +17843,16 @@
     </row>
     <row r="635" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A635" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="B635" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="C635" t="s">
-        <v>234</v>
+        <v>105</v>
       </c>
       <c r="D635" t="s">
-        <v>235</v>
+        <v>625</v>
       </c>
       <c r="E635" t="s">
         <v>15</v>
@@ -17844,10 +17861,10 @@
         <v>400</v>
       </c>
       <c r="G635">
-        <v>12.3</v>
+        <v>12.849600000000001</v>
       </c>
       <c r="H635">
-        <v>4</v>
+        <v>18</v>
       </c>
     </row>
     <row r="636" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
@@ -17881,10 +17898,10 @@
         <v>13</v>
       </c>
       <c r="C637" t="s">
-        <v>268</v>
+        <v>627</v>
       </c>
       <c r="D637" t="s">
-        <v>269</v>
+        <v>344</v>
       </c>
       <c r="E637" t="s">
         <v>15</v>
@@ -17896,7 +17913,7 @@
         <v>12.849600000000001</v>
       </c>
       <c r="H637">
-        <v>5</v>
+        <v>18</v>
       </c>
     </row>
     <row r="638" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
@@ -17907,10 +17924,10 @@
         <v>13</v>
       </c>
       <c r="C638" t="s">
-        <v>508</v>
+        <v>629</v>
       </c>
       <c r="D638" t="s">
-        <v>509</v>
+        <v>395</v>
       </c>
       <c r="E638" t="s">
         <v>15</v>
@@ -17922,7 +17939,7 @@
         <v>12.849600000000001</v>
       </c>
       <c r="H638">
-        <v>11</v>
+        <v>18</v>
       </c>
     </row>
     <row r="639" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
@@ -17948,7 +17965,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="640" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="640" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A640" t="s">
         <v>9</v>
       </c>
@@ -17973,16 +17990,16 @@
     </row>
     <row r="641" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A641" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="B641" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="C641" t="s">
-        <v>415</v>
+        <v>631</v>
       </c>
       <c r="D641" t="s">
-        <v>66</v>
+        <v>632</v>
       </c>
       <c r="E641" t="s">
         <v>15</v>
@@ -17991,10 +18008,10 @@
         <v>400</v>
       </c>
       <c r="G641">
-        <v>12.3</v>
+        <v>12.849600000000001</v>
       </c>
       <c r="H641">
-        <v>8</v>
+        <v>18</v>
       </c>
     </row>
     <row r="642" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
@@ -18094,16 +18111,16 @@
     </row>
     <row r="646" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A646" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="B646" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="C646" t="s">
-        <v>450</v>
+        <v>634</v>
       </c>
       <c r="D646" t="s">
-        <v>451</v>
+        <v>444</v>
       </c>
       <c r="E646" t="s">
         <v>15</v>
@@ -18112,10 +18129,10 @@
         <v>400</v>
       </c>
       <c r="G646">
-        <v>12.3</v>
+        <v>12.849600000000001</v>
       </c>
       <c r="H646">
-        <v>9</v>
+        <v>18</v>
       </c>
     </row>
     <row r="647" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
@@ -18149,10 +18166,10 @@
         <v>13</v>
       </c>
       <c r="C648" t="s">
-        <v>523</v>
+        <v>315</v>
       </c>
       <c r="D648" t="s">
-        <v>524</v>
+        <v>636</v>
       </c>
       <c r="E648" t="s">
         <v>15</v>
@@ -18164,7 +18181,7 @@
         <v>12.849600000000001</v>
       </c>
       <c r="H648">
-        <v>12</v>
+        <v>18</v>
       </c>
     </row>
     <row r="649" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
@@ -18265,7 +18282,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="653" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="653" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A653" t="s">
         <v>13</v>
       </c>
@@ -18293,16 +18310,16 @@
     </row>
     <row r="654" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A654" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="B654" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="C654" t="s">
-        <v>270</v>
+        <v>27</v>
       </c>
       <c r="D654" t="s">
-        <v>271</v>
+        <v>639</v>
       </c>
       <c r="E654" t="s">
         <v>15</v>
@@ -18311,10 +18328,10 @@
         <v>400</v>
       </c>
       <c r="G654">
-        <v>12.3</v>
+        <v>12.849600000000001</v>
       </c>
       <c r="H654">
-        <v>5</v>
+        <v>19</v>
       </c>
     </row>
     <row r="655" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
@@ -18348,10 +18365,10 @@
         <v>13</v>
       </c>
       <c r="C656" t="s">
-        <v>488</v>
+        <v>210</v>
       </c>
       <c r="D656" t="s">
-        <v>489</v>
+        <v>641</v>
       </c>
       <c r="E656" t="s">
         <v>15</v>
@@ -18363,7 +18380,7 @@
         <v>12.849600000000001</v>
       </c>
       <c r="H656">
-        <v>10</v>
+        <v>19</v>
       </c>
     </row>
     <row r="657" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
@@ -18417,16 +18434,16 @@
     </row>
     <row r="659" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A659" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="B659" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="C659" t="s">
-        <v>319</v>
+        <v>167</v>
       </c>
       <c r="D659" t="s">
-        <v>129</v>
+        <v>643</v>
       </c>
       <c r="E659" t="s">
         <v>15</v>
@@ -18435,10 +18452,10 @@
         <v>400</v>
       </c>
       <c r="G659">
-        <v>12.3</v>
+        <v>12.849600000000001</v>
       </c>
       <c r="H659">
-        <v>6</v>
+        <v>19</v>
       </c>
     </row>
     <row r="660" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
@@ -18538,16 +18555,16 @@
     </row>
     <row r="664" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A664" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="B664" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="C664" t="s">
-        <v>237</v>
+        <v>645</v>
       </c>
       <c r="D664" t="s">
-        <v>238</v>
+        <v>302</v>
       </c>
       <c r="E664" t="s">
         <v>15</v>
@@ -18556,10 +18573,10 @@
         <v>400</v>
       </c>
       <c r="G664">
-        <v>12.3</v>
+        <v>12.849600000000001</v>
       </c>
       <c r="H664">
-        <v>4</v>
+        <v>19</v>
       </c>
     </row>
     <row r="665" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
@@ -18570,10 +18587,10 @@
         <v>13</v>
       </c>
       <c r="C665" t="s">
-        <v>543</v>
+        <v>647</v>
       </c>
       <c r="D665" t="s">
-        <v>544</v>
+        <v>350</v>
       </c>
       <c r="E665" t="s">
         <v>15</v>
@@ -18585,7 +18602,7 @@
         <v>12.849600000000001</v>
       </c>
       <c r="H665">
-        <v>13</v>
+        <v>19</v>
       </c>
     </row>
     <row r="666" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
@@ -18634,7 +18651,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="668" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="668" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A668" t="s">
         <v>9</v>
       </c>
@@ -18680,7 +18697,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="670" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="670" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A670" t="s">
         <v>9</v>
       </c>
@@ -18757,16 +18774,16 @@
     </row>
     <row r="673" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A673" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="B673" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="C673" t="s">
-        <v>368</v>
+        <v>223</v>
       </c>
       <c r="D673" t="s">
-        <v>369</v>
+        <v>614</v>
       </c>
       <c r="E673" t="s">
         <v>15</v>
@@ -18775,10 +18792,10 @@
         <v>400</v>
       </c>
       <c r="G673">
-        <v>12.3</v>
+        <v>12.849600000000001</v>
       </c>
       <c r="H673">
-        <v>7</v>
+        <v>19</v>
       </c>
     </row>
     <row r="674" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
@@ -18947,16 +18964,16 @@
     </row>
     <row r="681" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A681" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="B681" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="C681" t="s">
-        <v>273</v>
+        <v>228</v>
       </c>
       <c r="D681" t="s">
-        <v>274</v>
+        <v>651</v>
       </c>
       <c r="E681" t="s">
         <v>15</v>
@@ -18965,10 +18982,10 @@
         <v>400</v>
       </c>
       <c r="G681">
-        <v>12.3</v>
+        <v>12.849600000000001</v>
       </c>
       <c r="H681">
-        <v>5</v>
+        <v>19</v>
       </c>
     </row>
     <row r="682" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
@@ -18994,7 +19011,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="683" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="683" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A683" t="s">
         <v>13</v>
       </c>
@@ -19040,7 +19057,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="685" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="685" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A685" t="s">
         <v>13</v>
       </c>
@@ -19164,7 +19181,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="690" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="690" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A690" t="s">
         <v>9</v>
       </c>
@@ -19213,7 +19230,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="692" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="692" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A692" t="s">
         <v>8</v>
       </c>
@@ -19261,16 +19278,16 @@
     </row>
     <row r="694" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A694" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="B694" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="C694" t="s">
-        <v>192</v>
+        <v>111</v>
       </c>
       <c r="D694" t="s">
-        <v>193</v>
+        <v>654</v>
       </c>
       <c r="E694" t="s">
         <v>15</v>
@@ -19279,10 +19296,10 @@
         <v>400</v>
       </c>
       <c r="G694">
-        <v>12.3</v>
+        <v>12.849600000000001</v>
       </c>
       <c r="H694">
-        <v>3</v>
+        <v>20</v>
       </c>
     </row>
     <row r="695" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
@@ -19360,7 +19377,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="698" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="698" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A698" t="s">
         <v>8</v>
       </c>
@@ -19406,7 +19423,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="700" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="700" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A700" t="s">
         <v>9</v>
       </c>
@@ -19481,7 +19498,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="703" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="703" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A703" t="s">
         <v>13</v>
       </c>
@@ -19550,7 +19567,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="706" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="706" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A706" t="s">
         <v>13</v>
       </c>
@@ -19599,7 +19616,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="708" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="708" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A708" t="s">
         <v>9</v>
       </c>
@@ -19694,7 +19711,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="712" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="712" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A712" t="s">
         <v>9</v>
       </c>
@@ -19769,7 +19786,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="715" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="715" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A715" t="s">
         <v>13</v>
       </c>
@@ -19792,7 +19809,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="716" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="716" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A716" t="s">
         <v>13</v>
       </c>
@@ -19841,7 +19858,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="718" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="718" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A718" t="s">
         <v>9</v>
       </c>
@@ -19913,7 +19930,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="721" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="721" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A721" t="s">
         <v>9</v>
       </c>
@@ -19941,19 +19958,11 @@
     </row>
   </sheetData>
   <autoFilter ref="A1:H721" xr:uid="{00000000-0001-0000-0000-000000000000}">
-    <filterColumn colId="5">
-      <filters>
-        <filter val="400"/>
-      </filters>
-    </filterColumn>
     <filterColumn colId="7">
       <filters>
         <filter val="1"/>
       </filters>
     </filterColumn>
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:H721">
-      <sortCondition ref="C1:C721"/>
-    </sortState>
   </autoFilter>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>